<commit_message>
added work to q7
</commit_message>
<xml_diff>
--- a/bls_electricity_prices.xlsx
+++ b/bls_electricity_prices.xlsx
@@ -23,13 +23,13 @@
     <t>Series Id:</t>
   </si>
   <si>
-    <t>APU000074714</t>
+    <t>APU000072610</t>
   </si>
   <si>
     <t>Series Title:</t>
   </si>
   <si>
-    <t>Gasoline, unleaded regular, per gallon/3.785 liters in U.S. city average, average price, not seasonally adjusted</t>
+    <t>Electricity per KWH in U.S. city average, average price, not seasonally adjusted</t>
   </si>
   <si>
     <t>Area:</t>
@@ -41,7 +41,7 @@
     <t>Item:</t>
   </si>
   <si>
-    <t>Gasoline, unleaded regular, per gallon/3.785 liters</t>
+    <t>Electricity per KWH</t>
   </si>
   <si>
     <t>Years:</t>
@@ -464,40 +464,40 @@
         <v>2022.0</v>
       </c>
       <c r="B11" t="n" s="14">
-        <v>3.413</v>
+        <v>0.147</v>
       </c>
       <c r="C11" t="n" s="14">
-        <v>3.592</v>
+        <v>0.148</v>
       </c>
       <c r="D11" t="n" s="14">
-        <v>4.312</v>
+        <v>0.15</v>
       </c>
       <c r="E11" t="n" s="14">
-        <v>4.271</v>
+        <v>0.151</v>
       </c>
       <c r="F11" t="n" s="14">
-        <v>4.604</v>
+        <v>0.154</v>
       </c>
       <c r="G11" t="n" s="14">
-        <v>5.058</v>
+        <v>0.16</v>
       </c>
       <c r="H11" t="n" s="14">
-        <v>4.667</v>
+        <v>0.164</v>
       </c>
       <c r="I11" t="n" s="14">
-        <v>4.101</v>
+        <v>0.167</v>
       </c>
       <c r="J11" t="n" s="14">
-        <v>3.881</v>
+        <v>0.167</v>
       </c>
       <c r="K11" t="n" s="14">
-        <v>4.016</v>
+        <v>0.166</v>
       </c>
       <c r="L11" t="n" s="14">
-        <v>3.853</v>
+        <v>0.163</v>
       </c>
       <c r="M11" t="n" s="14">
-        <v>3.356</v>
+        <v>0.165</v>
       </c>
     </row>
     <row r="10000"/>
@@ -516,7 +516,7 @@
   <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddHeader>&amp;CBureau of Labor Statistics</oddHeader>
-    <oddFooter>&amp;LSource: Bureau of Labor Statistics&amp;RGenerated on: December 10, 2023 (04:37:15 PM)</oddFooter>
+    <oddFooter>&amp;LSource: Bureau of Labor Statistics&amp;RGenerated on: December 10, 2023 (05:03:42 PM)</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>